<commit_message>
Finished RehabConcept DH paramter table and svg schematic.
</commit_message>
<xml_diff>
--- a/kinematics/DH_table.xlsx
+++ b/kinematics/DH_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t xml:space="preserve">Joint i</t>
   </si>
@@ -111,7 +111,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> [m]</t>
+      <t xml:space="preserve"> [cm]</t>
     </r>
   </si>
   <si>
@@ -141,14 +141,370 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> [m]</t>
-    </r>
+      <t xml:space="preserve"> [cm]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prismatic passive</t>
   </si>
   <si>
     <t xml:space="preserve">Base</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revolute active</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">pregledati predznake</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">dodati stupnjeve i pomake u promjenjive varijable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + 90</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - 90</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + 180</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + 90</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HandInteface</t>
   </si>
 </sst>
 </file>
@@ -243,13 +599,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -269,10 +637,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F5"/>
+  <dimension ref="B3:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,7 +648,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>0</v>
       </c>
@@ -296,27 +664,346 @@
       <c r="F3" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>36.68</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>5.69</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>14.72</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>12.22</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>9.46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix DH parameters, add each joint ROM, render RehabConcept with bones.
</commit_message>
<xml_diff>
--- a/kinematics/DH_table.xlsx
+++ b/kinematics/DH_table.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+  <si>
+    <t xml:space="preserve">ROM</t>
+  </si>
   <si>
     <t xml:space="preserve">Joint i</t>
   </si>
@@ -148,6 +151,12 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
+    <t xml:space="preserve">min [deg, cm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max [deg, cm]</t>
+  </si>
+  <si>
     <t xml:space="preserve">PP</t>
   </si>
   <si>
@@ -169,6 +178,15 @@
     <t xml:space="preserve">revolute active</t>
   </si>
   <si>
+    <t xml:space="preserve">Shoulder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revolute passive</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -190,7 +208,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">pregledati predznake</t>
+    <t xml:space="preserve">rom se odnosi na parametra u sljedećem stupcu</t>
   </si>
   <si>
     <r>
@@ -214,9 +232,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">dodati stupnjeve i pomake u promjenjive varijable</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -243,7 +258,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -257,14 +271,22 @@
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - 90</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -276,7 +298,15 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">6</t>
+      <t xml:space="preserve">6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">- 90</t>
     </r>
   </si>
   <si>
@@ -297,16 +327,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
+      <t xml:space="preserve">7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ 17,18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -320,6 +358,17 @@
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> + 90</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Elbow</t>
   </si>
   <si>
     <r>
@@ -343,6 +392,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Elbow-Wrist</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -364,11 +416,15 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
+    <t xml:space="preserve">Wrist</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -398,6 +454,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -427,6 +484,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -451,14 +509,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">RP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
+    <t xml:space="preserve">Wrist compensation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elastic hinge</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">θ</t>
     </r>
@@ -505,6 +567,9 @@
   </si>
   <si>
     <t xml:space="preserve">HandInteface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand interaction</t>
   </si>
 </sst>
 </file>
@@ -599,13 +664,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -637,376 +710,546 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:L19"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="L3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="4" t="n">
         <v>36.68</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="4" t="n">
         <v>31.4</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="4" t="n">
         <v>5.69</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>-120</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="4" t="n">
         <v>14.72</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="4" t="n">
         <v>3.83</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>-90</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="n">
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="4" t="n">
         <v>15.09</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>-90</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="n">
+      <c r="C10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>3.67</v>
+      <c r="E10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>-3.67</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>20</v>
+      <c r="C11" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>9.14</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>-120</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2" t="n">
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2" t="n">
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <v>12.22</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>-10</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="2" t="n">
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="4" t="n">
         <v>6.4</v>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>4.31</v>
+      <c r="F13" s="4" t="n">
+        <v>-4.31</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
+      <c r="C14" s="4" t="n">
+        <v>180</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="n">
         <v>9.46</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>23</v>
+      <c r="F14" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>-110</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="2" t="n">
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="4" t="n">
         <v>7.63</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="4" t="n">
         <v>10.31</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>-55</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="n">
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="n">
         <v>-90</v>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2" t="n">
+      <c r="E16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="n">
         <v>6.24</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>-30</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="n">
         <v>3.73</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="2" t="n">
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="n">
+      <c r="E18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
+      <c r="C19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="n">
         <v>10.49</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>29</v>
+      <c r="F19" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>